<commit_message>
Remove Marky Marc, and add flight details to reports
</commit_message>
<xml_diff>
--- a/sql/act.xlsx
+++ b/sql/act.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I31759\source\repos\BOSMAJ24\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCD062C-7D82-4198-8B37-83DD6674A043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DD8BC7-62B0-4D00-AFC4-73AF199B465D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="1995" windowWidth="21338" windowHeight="11422" xr2:uid="{6A94DAEF-3FB4-4FEE-B54A-43E7FD304352}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{6A94DAEF-3FB4-4FEE-B54A-43E7FD304352}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Flame Luconi</t>
   </si>
   <si>
-    <t>Marky Marc</t>
-  </si>
-  <si>
     <t>Gabriel HappyFeet</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
   </si>
   <si>
     <t>Qiosen &amp; Natalie</t>
-  </si>
-  <si>
-    <t>Andre</t>
   </si>
   <si>
     <t>Peynao &amp; Debora</t>
@@ -301,10 +295,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7460610E-3C31-4E1F-A627-9C56A73266EE}" name="Table1" displayName="Table1" ref="A1:D39" totalsRowShown="0">
-  <autoFilter ref="A1:D39" xr:uid="{7460610E-3C31-4E1F-A627-9C56A73266EE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D36">
-    <sortCondition ref="A2:A36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7460610E-3C31-4E1F-A627-9C56A73266EE}" name="Table1" displayName="Table1" ref="A1:D37" totalsRowShown="0">
+  <autoFilter ref="A1:D37" xr:uid="{7460610E-3C31-4E1F-A627-9C56A73266EE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D34">
+    <sortCondition ref="A2:A34"/>
   </sortState>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{94C3C80C-DB4B-4FA6-8C1D-5ABB437D91AA}" name="Name"/>
@@ -633,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CB071C-8639-415D-8B4F-FD65D30C1200}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -677,24 +671,24 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
       <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -702,10 +696,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -713,13 +710,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -727,13 +724,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -741,13 +738,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -755,10 +749,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -766,13 +763,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -780,13 +777,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -794,10 +788,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -805,13 +802,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -819,12 +816,9 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
         <v>53</v>
       </c>
       <c r="D14">
@@ -833,10 +827,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -844,24 +841,24 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
       <c r="D16">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -869,13 +866,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -883,13 +880,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -897,10 +891,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -908,10 +902,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -919,10 +913,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -930,13 +927,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -944,10 +938,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -955,10 +952,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -966,13 +963,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -980,10 +977,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -991,13 +988,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1005,10 +1002,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>55</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1016,13 +1016,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1030,13 +1027,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -1044,10 +1041,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1055,13 +1052,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -1069,10 +1063,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1080,10 +1074,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -1091,34 +1085,12 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38">
         <v>1</v>
       </c>
     </row>
@@ -1128,4 +1100,10 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{dd2e4901-b5ad-42ae-9e9d-f456e52148af}" enabled="1" method="Privileged" siteId="{3b07dc1f-22e7-4be1-ac66-a88bf3550222}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>